<commit_message>
Removed code for plotting the plant species NMDS
</commit_message>
<xml_diff>
--- a/PlantMatrix.xlsx
+++ b/PlantMatrix.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aurap\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\R\Moths_QuantReas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="48" windowWidth="20112" windowHeight="7992" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="48" windowWidth="20112" windowHeight="7992" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -1528,7 +1528,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -2084,48 +2084,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -2141,7 +2141,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Aura Alonso Rodriguez" refreshedDate="41661.525891898149" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="1290" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Aura Alonso Rodriguez" refreshedDate="41661.525891898149" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="1290">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:G1048576" sheet="tree list"/>
   </cacheSource>
@@ -14029,7 +14029,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:FH31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -14820,7 +14820,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -14895,23 +14895,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -14947,23 +14930,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -15139,14 +15105,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:FH31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.88671875" customWidth="1"/>
     <col min="2" max="2" width="16.33203125" customWidth="1"/>
@@ -21835,14 +21801,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G808"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="27" customWidth="1"/>
     <col min="6" max="6" width="25.21875" customWidth="1"/>
@@ -40444,14 +40410,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FH21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="5" customWidth="1"/>
@@ -50838,14 +50804,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="6" max="6" width="9.109375" style="5"/>
   </cols>
@@ -51907,14 +51873,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:15" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">

</xml_diff>

<commit_message>
Small edits to data files
</commit_message>
<xml_diff>
--- a/PlantMatrix.xlsx
+++ b/PlantMatrix.xlsx
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="125725"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId6"/>
+    <pivotCache cacheId="6" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -14029,7 +14029,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:FH31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -40414,7 +40414,7 @@
   <dimension ref="A1:FH21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -45860,13 +45860,13 @@
     </row>
     <row r="12" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B12" s="24">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -45884,7 +45884,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -45908,10 +45908,10 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
         <v>0</v>
@@ -46019,7 +46019,7 @@
         <v>0</v>
       </c>
       <c r="BB12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BC12">
         <v>0</v>
@@ -46091,7 +46091,7 @@
         <v>0</v>
       </c>
       <c r="BZ12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA12">
         <v>0</v>
@@ -46130,7 +46130,7 @@
         <v>0</v>
       </c>
       <c r="CM12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CN12">
         <v>0</v>
@@ -46268,7 +46268,7 @@
         <v>0</v>
       </c>
       <c r="EG12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="EH12">
         <v>0</v>
@@ -46354,13 +46354,13 @@
     </row>
     <row r="13" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B13" s="24">
         <v>2</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -46474,7 +46474,7 @@
         <v>0</v>
       </c>
       <c r="AO13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP13">
         <v>0</v>
@@ -46513,185 +46513,185 @@
         <v>0</v>
       </c>
       <c r="BB13">
+        <v>0</v>
+      </c>
+      <c r="BC13">
+        <v>0</v>
+      </c>
+      <c r="BD13">
+        <v>0</v>
+      </c>
+      <c r="BE13">
+        <v>1</v>
+      </c>
+      <c r="BF13">
+        <v>0</v>
+      </c>
+      <c r="BG13">
+        <v>0</v>
+      </c>
+      <c r="BH13">
+        <v>0</v>
+      </c>
+      <c r="BI13">
+        <v>0</v>
+      </c>
+      <c r="BJ13">
+        <v>0</v>
+      </c>
+      <c r="BK13">
+        <v>0</v>
+      </c>
+      <c r="BL13">
+        <v>0</v>
+      </c>
+      <c r="BM13">
+        <v>0</v>
+      </c>
+      <c r="BN13">
+        <v>0</v>
+      </c>
+      <c r="BO13">
+        <v>0</v>
+      </c>
+      <c r="BP13">
+        <v>0</v>
+      </c>
+      <c r="BQ13">
+        <v>0</v>
+      </c>
+      <c r="BR13">
+        <v>0</v>
+      </c>
+      <c r="BS13">
+        <v>0</v>
+      </c>
+      <c r="BT13">
+        <v>2</v>
+      </c>
+      <c r="BU13">
+        <v>0</v>
+      </c>
+      <c r="BV13">
+        <v>0</v>
+      </c>
+      <c r="BW13">
+        <v>0</v>
+      </c>
+      <c r="BX13">
+        <v>0</v>
+      </c>
+      <c r="BY13">
+        <v>0</v>
+      </c>
+      <c r="BZ13">
+        <v>0</v>
+      </c>
+      <c r="CA13">
+        <v>0</v>
+      </c>
+      <c r="CB13">
+        <v>0</v>
+      </c>
+      <c r="CC13">
+        <v>0</v>
+      </c>
+      <c r="CD13">
+        <v>0</v>
+      </c>
+      <c r="CE13">
+        <v>0</v>
+      </c>
+      <c r="CF13">
+        <v>0</v>
+      </c>
+      <c r="CG13">
+        <v>0</v>
+      </c>
+      <c r="CH13">
+        <v>0</v>
+      </c>
+      <c r="CI13">
+        <v>0</v>
+      </c>
+      <c r="CJ13">
+        <v>0</v>
+      </c>
+      <c r="CK13">
+        <v>0</v>
+      </c>
+      <c r="CL13">
+        <v>0</v>
+      </c>
+      <c r="CM13">
+        <v>2</v>
+      </c>
+      <c r="CN13">
+        <v>0</v>
+      </c>
+      <c r="CO13">
+        <v>0</v>
+      </c>
+      <c r="CP13">
+        <v>0</v>
+      </c>
+      <c r="CQ13">
+        <v>0</v>
+      </c>
+      <c r="CR13">
+        <v>0</v>
+      </c>
+      <c r="CS13">
+        <v>0</v>
+      </c>
+      <c r="CT13">
+        <v>0</v>
+      </c>
+      <c r="CU13">
+        <v>0</v>
+      </c>
+      <c r="CV13">
+        <v>0</v>
+      </c>
+      <c r="CW13">
+        <v>0</v>
+      </c>
+      <c r="CX13">
+        <v>0</v>
+      </c>
+      <c r="CY13">
+        <v>0</v>
+      </c>
+      <c r="CZ13">
+        <v>0</v>
+      </c>
+      <c r="DA13">
+        <v>0</v>
+      </c>
+      <c r="DB13">
+        <v>0</v>
+      </c>
+      <c r="DC13">
+        <v>0</v>
+      </c>
+      <c r="DD13">
+        <v>1</v>
+      </c>
+      <c r="DE13">
+        <v>0</v>
+      </c>
+      <c r="DF13">
+        <v>0</v>
+      </c>
+      <c r="DG13">
+        <v>0</v>
+      </c>
+      <c r="DH13">
+        <v>0</v>
+      </c>
+      <c r="DI13">
         <v>5</v>
       </c>
-      <c r="BC13">
-        <v>0</v>
-      </c>
-      <c r="BD13">
-        <v>0</v>
-      </c>
-      <c r="BE13">
-        <v>0</v>
-      </c>
-      <c r="BF13">
-        <v>0</v>
-      </c>
-      <c r="BG13">
-        <v>0</v>
-      </c>
-      <c r="BH13">
-        <v>0</v>
-      </c>
-      <c r="BI13">
-        <v>0</v>
-      </c>
-      <c r="BJ13">
-        <v>0</v>
-      </c>
-      <c r="BK13">
-        <v>0</v>
-      </c>
-      <c r="BL13">
-        <v>0</v>
-      </c>
-      <c r="BM13">
-        <v>0</v>
-      </c>
-      <c r="BN13">
-        <v>0</v>
-      </c>
-      <c r="BO13">
-        <v>0</v>
-      </c>
-      <c r="BP13">
-        <v>0</v>
-      </c>
-      <c r="BQ13">
-        <v>0</v>
-      </c>
-      <c r="BR13">
-        <v>0</v>
-      </c>
-      <c r="BS13">
-        <v>0</v>
-      </c>
-      <c r="BT13">
-        <v>0</v>
-      </c>
-      <c r="BU13">
-        <v>0</v>
-      </c>
-      <c r="BV13">
-        <v>0</v>
-      </c>
-      <c r="BW13">
-        <v>0</v>
-      </c>
-      <c r="BX13">
-        <v>0</v>
-      </c>
-      <c r="BY13">
-        <v>0</v>
-      </c>
-      <c r="BZ13">
-        <v>0</v>
-      </c>
-      <c r="CA13">
-        <v>0</v>
-      </c>
-      <c r="CB13">
-        <v>0</v>
-      </c>
-      <c r="CC13">
-        <v>0</v>
-      </c>
-      <c r="CD13">
-        <v>0</v>
-      </c>
-      <c r="CE13">
-        <v>0</v>
-      </c>
-      <c r="CF13">
-        <v>0</v>
-      </c>
-      <c r="CG13">
-        <v>0</v>
-      </c>
-      <c r="CH13">
-        <v>0</v>
-      </c>
-      <c r="CI13">
-        <v>0</v>
-      </c>
-      <c r="CJ13">
-        <v>0</v>
-      </c>
-      <c r="CK13">
-        <v>0</v>
-      </c>
-      <c r="CL13">
-        <v>0</v>
-      </c>
-      <c r="CM13">
-        <v>0</v>
-      </c>
-      <c r="CN13">
-        <v>0</v>
-      </c>
-      <c r="CO13">
-        <v>0</v>
-      </c>
-      <c r="CP13">
-        <v>0</v>
-      </c>
-      <c r="CQ13">
-        <v>0</v>
-      </c>
-      <c r="CR13">
-        <v>0</v>
-      </c>
-      <c r="CS13">
-        <v>0</v>
-      </c>
-      <c r="CT13">
-        <v>0</v>
-      </c>
-      <c r="CU13">
-        <v>0</v>
-      </c>
-      <c r="CV13">
-        <v>0</v>
-      </c>
-      <c r="CW13">
-        <v>0</v>
-      </c>
-      <c r="CX13">
-        <v>0</v>
-      </c>
-      <c r="CY13">
-        <v>0</v>
-      </c>
-      <c r="CZ13">
-        <v>0</v>
-      </c>
-      <c r="DA13">
-        <v>0</v>
-      </c>
-      <c r="DB13">
-        <v>0</v>
-      </c>
-      <c r="DC13">
-        <v>0</v>
-      </c>
-      <c r="DD13">
-        <v>0</v>
-      </c>
-      <c r="DE13">
-        <v>0</v>
-      </c>
-      <c r="DF13">
-        <v>0</v>
-      </c>
-      <c r="DG13">
-        <v>0</v>
-      </c>
-      <c r="DH13">
-        <v>0</v>
-      </c>
-      <c r="DI13">
-        <v>0</v>
-      </c>
       <c r="DJ13">
         <v>0</v>
       </c>
@@ -46816,7 +46816,7 @@
         <v>0</v>
       </c>
       <c r="EY13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EZ13">
         <v>0</v>
@@ -46828,7 +46828,7 @@
         <v>0</v>
       </c>
       <c r="FC13">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="FD13">
         <v>0</v>
@@ -46848,13 +46848,13 @@
     </row>
     <row r="14" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B14" s="24">
         <v>3</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -46869,7 +46869,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -46884,13 +46884,13 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <v>0</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P14">
         <v>0</v>
@@ -46917,19 +46917,19 @@
         <v>0</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y14">
         <v>0</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14">
         <v>0</v>
@@ -46944,7 +46944,7 @@
         <v>0</v>
       </c>
       <c r="AG14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AH14">
         <v>0</v>
@@ -46983,7 +46983,7 @@
         <v>0</v>
       </c>
       <c r="AT14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AU14">
         <v>0</v>
@@ -47007,32 +47007,32 @@
         <v>0</v>
       </c>
       <c r="BB14">
+        <v>0</v>
+      </c>
+      <c r="BC14">
+        <v>0</v>
+      </c>
+      <c r="BD14">
+        <v>0</v>
+      </c>
+      <c r="BE14">
+        <v>2</v>
+      </c>
+      <c r="BF14">
+        <v>0</v>
+      </c>
+      <c r="BG14">
+        <v>0</v>
+      </c>
+      <c r="BH14">
+        <v>0</v>
+      </c>
+      <c r="BI14">
+        <v>2</v>
+      </c>
+      <c r="BJ14">
         <v>4</v>
       </c>
-      <c r="BC14">
-        <v>0</v>
-      </c>
-      <c r="BD14">
-        <v>0</v>
-      </c>
-      <c r="BE14">
-        <v>0</v>
-      </c>
-      <c r="BF14">
-        <v>0</v>
-      </c>
-      <c r="BG14">
-        <v>0</v>
-      </c>
-      <c r="BH14">
-        <v>0</v>
-      </c>
-      <c r="BI14">
-        <v>0</v>
-      </c>
-      <c r="BJ14">
-        <v>0</v>
-      </c>
       <c r="BK14">
         <v>0</v>
       </c>
@@ -47046,7 +47046,7 @@
         <v>0</v>
       </c>
       <c r="BO14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BP14">
         <v>0</v>
@@ -47061,10 +47061,10 @@
         <v>0</v>
       </c>
       <c r="BT14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BU14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BV14">
         <v>0</v>
@@ -47073,7 +47073,7 @@
         <v>0</v>
       </c>
       <c r="BX14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BY14">
         <v>0</v>
@@ -47094,7 +47094,7 @@
         <v>0</v>
       </c>
       <c r="CE14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="CF14">
         <v>0</v>
@@ -47106,7 +47106,7 @@
         <v>0</v>
       </c>
       <c r="CI14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CJ14">
         <v>0</v>
@@ -47118,7 +47118,7 @@
         <v>0</v>
       </c>
       <c r="CM14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN14">
         <v>0</v>
@@ -47160,7 +47160,7 @@
         <v>0</v>
       </c>
       <c r="DA14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DB14">
         <v>0</v>
@@ -47169,7 +47169,7 @@
         <v>0</v>
       </c>
       <c r="DD14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DE14">
         <v>0</v>
@@ -47184,7 +47184,7 @@
         <v>0</v>
       </c>
       <c r="DI14">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="DJ14">
         <v>0</v>
@@ -47214,7 +47214,7 @@
         <v>0</v>
       </c>
       <c r="DS14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DT14">
         <v>0</v>
@@ -47226,7 +47226,7 @@
         <v>0</v>
       </c>
       <c r="DW14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DX14">
         <v>0</v>
@@ -47307,7 +47307,7 @@
         <v>0</v>
       </c>
       <c r="EX14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="EY14">
         <v>0</v>
@@ -47316,7 +47316,7 @@
         <v>0</v>
       </c>
       <c r="FA14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="FB14">
         <v>0</v>
@@ -47342,13 +47342,13 @@
     </row>
     <row r="15" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B15" s="24">
         <v>4</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -47438,7 +47438,7 @@
         <v>0</v>
       </c>
       <c r="AG15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH15">
         <v>0</v>
@@ -47462,7 +47462,7 @@
         <v>0</v>
       </c>
       <c r="AO15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AP15">
         <v>0</v>
@@ -47495,98 +47495,98 @@
         <v>0</v>
       </c>
       <c r="AZ15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA15">
         <v>0</v>
       </c>
       <c r="BB15">
+        <v>0</v>
+      </c>
+      <c r="BC15">
+        <v>0</v>
+      </c>
+      <c r="BD15">
+        <v>0</v>
+      </c>
+      <c r="BE15">
+        <v>0</v>
+      </c>
+      <c r="BF15">
+        <v>0</v>
+      </c>
+      <c r="BG15">
+        <v>0</v>
+      </c>
+      <c r="BH15">
+        <v>0</v>
+      </c>
+      <c r="BI15">
+        <v>0</v>
+      </c>
+      <c r="BJ15">
+        <v>0</v>
+      </c>
+      <c r="BK15">
+        <v>0</v>
+      </c>
+      <c r="BL15">
+        <v>0</v>
+      </c>
+      <c r="BM15">
+        <v>0</v>
+      </c>
+      <c r="BN15">
+        <v>0</v>
+      </c>
+      <c r="BO15">
+        <v>0</v>
+      </c>
+      <c r="BP15">
+        <v>0</v>
+      </c>
+      <c r="BQ15">
+        <v>0</v>
+      </c>
+      <c r="BR15">
+        <v>0</v>
+      </c>
+      <c r="BS15">
+        <v>0</v>
+      </c>
+      <c r="BT15">
+        <v>0</v>
+      </c>
+      <c r="BU15">
+        <v>0</v>
+      </c>
+      <c r="BV15">
+        <v>0</v>
+      </c>
+      <c r="BW15">
+        <v>0</v>
+      </c>
+      <c r="BX15">
+        <v>0</v>
+      </c>
+      <c r="BY15">
+        <v>0</v>
+      </c>
+      <c r="BZ15">
+        <v>0</v>
+      </c>
+      <c r="CA15">
+        <v>0</v>
+      </c>
+      <c r="CB15">
+        <v>0</v>
+      </c>
+      <c r="CC15">
+        <v>0</v>
+      </c>
+      <c r="CD15">
         <v>4</v>
       </c>
-      <c r="BC15">
-        <v>0</v>
-      </c>
-      <c r="BD15">
-        <v>0</v>
-      </c>
-      <c r="BE15">
-        <v>0</v>
-      </c>
-      <c r="BF15">
-        <v>0</v>
-      </c>
-      <c r="BG15">
-        <v>0</v>
-      </c>
-      <c r="BH15">
-        <v>0</v>
-      </c>
-      <c r="BI15">
-        <v>0</v>
-      </c>
-      <c r="BJ15">
-        <v>0</v>
-      </c>
-      <c r="BK15">
-        <v>0</v>
-      </c>
-      <c r="BL15">
-        <v>0</v>
-      </c>
-      <c r="BM15">
-        <v>0</v>
-      </c>
-      <c r="BN15">
-        <v>0</v>
-      </c>
-      <c r="BO15">
-        <v>0</v>
-      </c>
-      <c r="BP15">
-        <v>0</v>
-      </c>
-      <c r="BQ15">
-        <v>0</v>
-      </c>
-      <c r="BR15">
-        <v>0</v>
-      </c>
-      <c r="BS15">
-        <v>0</v>
-      </c>
-      <c r="BT15">
-        <v>0</v>
-      </c>
-      <c r="BU15">
-        <v>0</v>
-      </c>
-      <c r="BV15">
-        <v>0</v>
-      </c>
-      <c r="BW15">
-        <v>0</v>
-      </c>
-      <c r="BX15">
-        <v>0</v>
-      </c>
-      <c r="BY15">
-        <v>0</v>
-      </c>
-      <c r="BZ15">
-        <v>0</v>
-      </c>
-      <c r="CA15">
-        <v>0</v>
-      </c>
-      <c r="CB15">
-        <v>0</v>
-      </c>
-      <c r="CC15">
-        <v>0</v>
-      </c>
-      <c r="CD15">
-        <v>0</v>
-      </c>
       <c r="CE15">
         <v>0</v>
       </c>
@@ -47612,7 +47612,7 @@
         <v>0</v>
       </c>
       <c r="CM15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CN15">
         <v>0</v>
@@ -47741,7 +47741,7 @@
         <v>0</v>
       </c>
       <c r="ED15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EE15">
         <v>0</v>
@@ -47750,7 +47750,7 @@
         <v>0</v>
       </c>
       <c r="EG15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EH15">
         <v>0</v>
@@ -47804,7 +47804,7 @@
         <v>0</v>
       </c>
       <c r="EY15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="EZ15">
         <v>0</v>
@@ -47816,7 +47816,7 @@
         <v>0</v>
       </c>
       <c r="FC15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="FD15">
         <v>0</v>
@@ -47825,7 +47825,7 @@
         <v>0</v>
       </c>
       <c r="FF15">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="FG15">
         <v>0</v>
@@ -47836,19 +47836,19 @@
     </row>
     <row r="16" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="B16" s="24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -47878,7 +47878,7 @@
         <v>0</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -47911,16 +47911,16 @@
         <v>0</v>
       </c>
       <c r="Z16">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="AA16">
         <v>0</v>
       </c>
       <c r="AB16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AD16">
         <v>0</v>
@@ -47929,10 +47929,10 @@
         <v>0</v>
       </c>
       <c r="AF16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH16">
         <v>0</v>
@@ -47956,13 +47956,13 @@
         <v>0</v>
       </c>
       <c r="AO16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AP16">
         <v>0</v>
       </c>
       <c r="AQ16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR16">
         <v>0</v>
@@ -47995,167 +47995,167 @@
         <v>0</v>
       </c>
       <c r="BB16">
+        <v>0</v>
+      </c>
+      <c r="BC16">
+        <v>0</v>
+      </c>
+      <c r="BD16">
+        <v>0</v>
+      </c>
+      <c r="BE16">
+        <v>0</v>
+      </c>
+      <c r="BF16">
+        <v>0</v>
+      </c>
+      <c r="BG16">
+        <v>0</v>
+      </c>
+      <c r="BH16">
+        <v>0</v>
+      </c>
+      <c r="BI16">
+        <v>0</v>
+      </c>
+      <c r="BJ16">
+        <v>0</v>
+      </c>
+      <c r="BK16">
+        <v>0</v>
+      </c>
+      <c r="BL16">
+        <v>0</v>
+      </c>
+      <c r="BM16">
+        <v>0</v>
+      </c>
+      <c r="BN16">
+        <v>0</v>
+      </c>
+      <c r="BO16">
+        <v>0</v>
+      </c>
+      <c r="BP16">
+        <v>44</v>
+      </c>
+      <c r="BQ16">
+        <v>0</v>
+      </c>
+      <c r="BR16">
+        <v>1</v>
+      </c>
+      <c r="BS16">
+        <v>0</v>
+      </c>
+      <c r="BT16">
+        <v>34</v>
+      </c>
+      <c r="BU16">
+        <v>0</v>
+      </c>
+      <c r="BV16">
+        <v>0</v>
+      </c>
+      <c r="BW16">
+        <v>2</v>
+      </c>
+      <c r="BX16">
+        <v>0</v>
+      </c>
+      <c r="BY16">
+        <v>0</v>
+      </c>
+      <c r="BZ16">
+        <v>0</v>
+      </c>
+      <c r="CA16">
+        <v>0</v>
+      </c>
+      <c r="CB16">
+        <v>0</v>
+      </c>
+      <c r="CC16">
+        <v>0</v>
+      </c>
+      <c r="CD16">
+        <v>0</v>
+      </c>
+      <c r="CE16">
+        <v>0</v>
+      </c>
+      <c r="CF16">
+        <v>0</v>
+      </c>
+      <c r="CG16">
+        <v>0</v>
+      </c>
+      <c r="CH16">
+        <v>1</v>
+      </c>
+      <c r="CI16">
+        <v>0</v>
+      </c>
+      <c r="CJ16">
+        <v>0</v>
+      </c>
+      <c r="CK16">
+        <v>0</v>
+      </c>
+      <c r="CL16">
+        <v>0</v>
+      </c>
+      <c r="CM16">
+        <v>0</v>
+      </c>
+      <c r="CN16">
+        <v>0</v>
+      </c>
+      <c r="CO16">
+        <v>0</v>
+      </c>
+      <c r="CP16">
+        <v>14</v>
+      </c>
+      <c r="CQ16">
+        <v>0</v>
+      </c>
+      <c r="CR16">
+        <v>0</v>
+      </c>
+      <c r="CS16">
+        <v>0</v>
+      </c>
+      <c r="CT16">
+        <v>0</v>
+      </c>
+      <c r="CU16">
+        <v>0</v>
+      </c>
+      <c r="CV16">
+        <v>0</v>
+      </c>
+      <c r="CW16">
+        <v>0</v>
+      </c>
+      <c r="CX16">
+        <v>0</v>
+      </c>
+      <c r="CY16">
+        <v>0</v>
+      </c>
+      <c r="CZ16">
+        <v>0</v>
+      </c>
+      <c r="DA16">
+        <v>0</v>
+      </c>
+      <c r="DB16">
+        <v>0</v>
+      </c>
+      <c r="DC16">
         <v>4</v>
       </c>
-      <c r="BC16">
-        <v>0</v>
-      </c>
-      <c r="BD16">
-        <v>0</v>
-      </c>
-      <c r="BE16">
-        <v>0</v>
-      </c>
-      <c r="BF16">
-        <v>0</v>
-      </c>
-      <c r="BG16">
-        <v>0</v>
-      </c>
-      <c r="BH16">
-        <v>0</v>
-      </c>
-      <c r="BI16">
-        <v>0</v>
-      </c>
-      <c r="BJ16">
-        <v>0</v>
-      </c>
-      <c r="BK16">
-        <v>0</v>
-      </c>
-      <c r="BL16">
-        <v>0</v>
-      </c>
-      <c r="BM16">
-        <v>0</v>
-      </c>
-      <c r="BN16">
-        <v>0</v>
-      </c>
-      <c r="BO16">
-        <v>0</v>
-      </c>
-      <c r="BP16">
-        <v>0</v>
-      </c>
-      <c r="BQ16">
-        <v>0</v>
-      </c>
-      <c r="BR16">
-        <v>0</v>
-      </c>
-      <c r="BS16">
-        <v>0</v>
-      </c>
-      <c r="BT16">
-        <v>0</v>
-      </c>
-      <c r="BU16">
-        <v>0</v>
-      </c>
-      <c r="BV16">
-        <v>0</v>
-      </c>
-      <c r="BW16">
-        <v>0</v>
-      </c>
-      <c r="BX16">
-        <v>0</v>
-      </c>
-      <c r="BY16">
-        <v>0</v>
-      </c>
-      <c r="BZ16">
-        <v>0</v>
-      </c>
-      <c r="CA16">
-        <v>0</v>
-      </c>
-      <c r="CB16">
-        <v>0</v>
-      </c>
-      <c r="CC16">
-        <v>0</v>
-      </c>
-      <c r="CD16">
-        <v>0</v>
-      </c>
-      <c r="CE16">
-        <v>0</v>
-      </c>
-      <c r="CF16">
-        <v>0</v>
-      </c>
-      <c r="CG16">
-        <v>0</v>
-      </c>
-      <c r="CH16">
-        <v>0</v>
-      </c>
-      <c r="CI16">
-        <v>0</v>
-      </c>
-      <c r="CJ16">
-        <v>0</v>
-      </c>
-      <c r="CK16">
-        <v>0</v>
-      </c>
-      <c r="CL16">
-        <v>0</v>
-      </c>
-      <c r="CM16">
-        <v>0</v>
-      </c>
-      <c r="CN16">
-        <v>0</v>
-      </c>
-      <c r="CO16">
-        <v>0</v>
-      </c>
-      <c r="CP16">
-        <v>0</v>
-      </c>
-      <c r="CQ16">
-        <v>0</v>
-      </c>
-      <c r="CR16">
-        <v>0</v>
-      </c>
-      <c r="CS16">
-        <v>0</v>
-      </c>
-      <c r="CT16">
-        <v>0</v>
-      </c>
-      <c r="CU16">
-        <v>0</v>
-      </c>
-      <c r="CV16">
-        <v>0</v>
-      </c>
-      <c r="CW16">
-        <v>0</v>
-      </c>
-      <c r="CX16">
-        <v>0</v>
-      </c>
-      <c r="CY16">
-        <v>0</v>
-      </c>
-      <c r="CZ16">
-        <v>0</v>
-      </c>
-      <c r="DA16">
-        <v>0</v>
-      </c>
-      <c r="DB16">
-        <v>0</v>
-      </c>
-      <c r="DC16">
-        <v>0</v>
-      </c>
       <c r="DD16">
         <v>0</v>
       </c>
@@ -48193,7 +48193,7 @@
         <v>0</v>
       </c>
       <c r="DP16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DQ16">
         <v>0</v>
@@ -48214,7 +48214,7 @@
         <v>0</v>
       </c>
       <c r="DW16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="DX16">
         <v>0</v>
@@ -48295,7 +48295,7 @@
         <v>0</v>
       </c>
       <c r="EX16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="EY16">
         <v>0</v>
@@ -48310,7 +48310,7 @@
         <v>0</v>
       </c>
       <c r="FC16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="FD16">
         <v>0</v>
@@ -48330,13 +48330,13 @@
     </row>
     <row r="17" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B17" s="24">
         <v>1</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -48354,7 +48354,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -48378,10 +48378,10 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S17">
         <v>0</v>
@@ -48489,7 +48489,7 @@
         <v>0</v>
       </c>
       <c r="BB17">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BC17">
         <v>0</v>
@@ -48561,7 +48561,7 @@
         <v>0</v>
       </c>
       <c r="BZ17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA17">
         <v>0</v>
@@ -48600,7 +48600,7 @@
         <v>0</v>
       </c>
       <c r="CM17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="CN17">
         <v>0</v>
@@ -48738,7 +48738,7 @@
         <v>0</v>
       </c>
       <c r="EG17">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="EH17">
         <v>0</v>
@@ -48824,13 +48824,13 @@
     </row>
     <row r="18" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B18" s="24">
         <v>2</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -48944,7 +48944,7 @@
         <v>0</v>
       </c>
       <c r="AO18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP18">
         <v>0</v>
@@ -48983,7 +48983,7 @@
         <v>0</v>
       </c>
       <c r="BB18">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="BC18">
         <v>0</v>
@@ -48992,7 +48992,7 @@
         <v>0</v>
       </c>
       <c r="BE18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF18">
         <v>0</v>
@@ -49037,7 +49037,7 @@
         <v>0</v>
       </c>
       <c r="BT18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BU18">
         <v>0</v>
@@ -49094,7 +49094,7 @@
         <v>0</v>
       </c>
       <c r="CM18">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="CN18">
         <v>0</v>
@@ -49145,7 +49145,7 @@
         <v>0</v>
       </c>
       <c r="DD18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DE18">
         <v>0</v>
@@ -49160,7 +49160,7 @@
         <v>0</v>
       </c>
       <c r="DI18">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="DJ18">
         <v>0</v>
@@ -49286,7 +49286,7 @@
         <v>0</v>
       </c>
       <c r="EY18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EZ18">
         <v>0</v>
@@ -49298,7 +49298,7 @@
         <v>0</v>
       </c>
       <c r="FC18">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="FD18">
         <v>0</v>
@@ -49318,13 +49318,13 @@
     </row>
     <row r="19" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B19" s="24">
         <v>3</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -49339,7 +49339,7 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -49354,13 +49354,13 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
       <c r="O19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P19">
         <v>0</v>
@@ -49387,19 +49387,19 @@
         <v>0</v>
       </c>
       <c r="X19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y19">
         <v>0</v>
       </c>
       <c r="Z19">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AA19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC19">
         <v>0</v>
@@ -49414,7 +49414,7 @@
         <v>0</v>
       </c>
       <c r="AG19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH19">
         <v>0</v>
@@ -49453,7 +49453,7 @@
         <v>0</v>
       </c>
       <c r="AT19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AU19">
         <v>0</v>
@@ -49477,7 +49477,7 @@
         <v>0</v>
       </c>
       <c r="BB19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BC19">
         <v>0</v>
@@ -49486,7 +49486,7 @@
         <v>0</v>
       </c>
       <c r="BE19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BF19">
         <v>0</v>
@@ -49498,10 +49498,10 @@
         <v>0</v>
       </c>
       <c r="BI19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BJ19">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BK19">
         <v>0</v>
@@ -49516,7 +49516,7 @@
         <v>0</v>
       </c>
       <c r="BO19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BP19">
         <v>0</v>
@@ -49531,10 +49531,10 @@
         <v>0</v>
       </c>
       <c r="BT19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BU19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BV19">
         <v>0</v>
@@ -49543,7 +49543,7 @@
         <v>0</v>
       </c>
       <c r="BX19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BY19">
         <v>0</v>
@@ -49564,7 +49564,7 @@
         <v>0</v>
       </c>
       <c r="CE19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="CF19">
         <v>0</v>
@@ -49576,7 +49576,7 @@
         <v>0</v>
       </c>
       <c r="CI19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="CJ19">
         <v>0</v>
@@ -49588,7 +49588,7 @@
         <v>0</v>
       </c>
       <c r="CM19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CN19">
         <v>0</v>
@@ -49630,7 +49630,7 @@
         <v>0</v>
       </c>
       <c r="DA19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DB19">
         <v>0</v>
@@ -49639,7 +49639,7 @@
         <v>0</v>
       </c>
       <c r="DD19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DE19">
         <v>0</v>
@@ -49654,7 +49654,7 @@
         <v>0</v>
       </c>
       <c r="DI19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="DJ19">
         <v>0</v>
@@ -49684,7 +49684,7 @@
         <v>0</v>
       </c>
       <c r="DS19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DT19">
         <v>0</v>
@@ -49696,7 +49696,7 @@
         <v>0</v>
       </c>
       <c r="DW19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DX19">
         <v>0</v>
@@ -49777,7 +49777,7 @@
         <v>0</v>
       </c>
       <c r="EX19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="EY19">
         <v>0</v>
@@ -49786,7 +49786,7 @@
         <v>0</v>
       </c>
       <c r="FA19">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="FB19">
         <v>0</v>
@@ -49812,13 +49812,13 @@
     </row>
     <row r="20" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B20" s="24">
         <v>4</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -49908,7 +49908,7 @@
         <v>0</v>
       </c>
       <c r="AG20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH20">
         <v>0</v>
@@ -49932,7 +49932,7 @@
         <v>0</v>
       </c>
       <c r="AO20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AP20">
         <v>0</v>
@@ -49965,13 +49965,13 @@
         <v>0</v>
       </c>
       <c r="AZ20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BA20">
         <v>0</v>
       </c>
       <c r="BB20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BC20">
         <v>0</v>
@@ -50055,7 +50055,7 @@
         <v>0</v>
       </c>
       <c r="CD20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="CE20">
         <v>0</v>
@@ -50082,7 +50082,7 @@
         <v>0</v>
       </c>
       <c r="CM20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="CN20">
         <v>0</v>
@@ -50211,7 +50211,7 @@
         <v>0</v>
       </c>
       <c r="ED20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EE20">
         <v>0</v>
@@ -50220,7 +50220,7 @@
         <v>0</v>
       </c>
       <c r="EG20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EH20">
         <v>0</v>
@@ -50274,7 +50274,7 @@
         <v>0</v>
       </c>
       <c r="EY20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="EZ20">
         <v>0</v>
@@ -50286,7 +50286,7 @@
         <v>0</v>
       </c>
       <c r="FC20">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="FD20">
         <v>0</v>
@@ -50295,7 +50295,7 @@
         <v>0</v>
       </c>
       <c r="FF20">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="FG20">
         <v>0</v>
@@ -50306,19 +50306,19 @@
     </row>
     <row r="21" spans="1:164" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B21" s="24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -50348,7 +50348,7 @@
         <v>0</v>
       </c>
       <c r="O21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P21">
         <v>0</v>
@@ -50381,16 +50381,16 @@
         <v>0</v>
       </c>
       <c r="Z21">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="AA21">
         <v>0</v>
       </c>
       <c r="AB21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AD21">
         <v>0</v>
@@ -50399,10 +50399,10 @@
         <v>0</v>
       </c>
       <c r="AF21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH21">
         <v>0</v>
@@ -50426,13 +50426,13 @@
         <v>0</v>
       </c>
       <c r="AO21">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AP21">
         <v>0</v>
       </c>
       <c r="AQ21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AR21">
         <v>0</v>
@@ -50465,7 +50465,7 @@
         <v>0</v>
       </c>
       <c r="BB21">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BC21">
         <v>0</v>
@@ -50507,19 +50507,19 @@
         <v>0</v>
       </c>
       <c r="BP21">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="BQ21">
         <v>0</v>
       </c>
       <c r="BR21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS21">
         <v>0</v>
       </c>
       <c r="BT21">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="BU21">
         <v>0</v>
@@ -50528,7 +50528,7 @@
         <v>0</v>
       </c>
       <c r="BW21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BX21">
         <v>0</v>
@@ -50561,7 +50561,7 @@
         <v>0</v>
       </c>
       <c r="CH21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI21">
         <v>0</v>
@@ -50585,7 +50585,7 @@
         <v>0</v>
       </c>
       <c r="CP21">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="CQ21">
         <v>0</v>
@@ -50624,7 +50624,7 @@
         <v>0</v>
       </c>
       <c r="DC21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="DD21">
         <v>0</v>
@@ -50663,7 +50663,7 @@
         <v>0</v>
       </c>
       <c r="DP21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DQ21">
         <v>0</v>
@@ -50684,7 +50684,7 @@
         <v>0</v>
       </c>
       <c r="DW21">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DX21">
         <v>0</v>
@@ -50765,7 +50765,7 @@
         <v>0</v>
       </c>
       <c r="EX21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="EY21">
         <v>0</v>
@@ -50780,7 +50780,7 @@
         <v>0</v>
       </c>
       <c r="FC21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="FD21">
         <v>0</v>

</xml_diff>